<commit_message>
sistemate le descrittive e altre cosette
</commit_message>
<xml_diff>
--- a/output/risultati.xlsx
+++ b/output/risultati.xlsx
@@ -440,22 +440,22 @@
         <v>1276</v>
       </c>
       <c r="C2" t="n">
-        <v>5233.01724137931</v>
+        <v>5262.81347962382</v>
       </c>
       <c r="D2" t="n">
-        <v>4262.08384328286</v>
+        <v>4281.84807490595</v>
       </c>
       <c r="E2" t="n">
-        <v>6203.95063947577</v>
+        <v>6243.7788843417</v>
       </c>
       <c r="F2" t="n">
-        <v>55.7592118006328</v>
+        <v>54.5239802822583</v>
       </c>
       <c r="G2" t="n">
-        <v>45.2329706088816</v>
+        <v>44.2375577066344</v>
       </c>
       <c r="H2" t="n">
-        <v>67.0483772317106</v>
+        <v>65.5439877236182</v>
       </c>
     </row>
     <row r="3">
@@ -466,22 +466,22 @@
         <v>112</v>
       </c>
       <c r="C3" t="n">
-        <v>5437.89285714286</v>
+        <v>6038.24107142857</v>
       </c>
       <c r="D3" t="n">
-        <v>1826.03551084252</v>
+        <v>2546.52968249249</v>
       </c>
       <c r="E3" t="n">
-        <v>9049.75020344319</v>
+        <v>9529.95246036466</v>
       </c>
       <c r="F3" t="n">
-        <v>36.0150500869684</v>
+        <v>37.4098787139257</v>
       </c>
       <c r="G3" t="n">
-        <v>12.3175006903326</v>
+        <v>13.7963507038835</v>
       </c>
       <c r="H3" t="n">
-        <v>64.7124778992955</v>
+        <v>65.92337672856</v>
       </c>
     </row>
     <row r="4">
@@ -492,22 +492,22 @@
         <v>216</v>
       </c>
       <c r="C4" t="n">
-        <v>5068.98148148148</v>
+        <v>5396.43518518519</v>
       </c>
       <c r="D4" t="n">
-        <v>2065.44608037724</v>
+        <v>2447.53158962581</v>
       </c>
       <c r="E4" t="n">
-        <v>8072.51688258572</v>
+        <v>8345.33878074456</v>
       </c>
       <c r="F4" t="n">
-        <v>44.87066664271</v>
+        <v>43.0402354120618</v>
       </c>
       <c r="G4" t="n">
-        <v>23.1057892059003</v>
+        <v>20.5138173773102</v>
       </c>
       <c r="H4" t="n">
-        <v>70.4835344372034</v>
+        <v>69.7772868871902</v>
       </c>
     </row>
     <row r="5">
@@ -518,22 +518,22 @@
         <v>35</v>
       </c>
       <c r="C5" t="n">
-        <v>5014.85714285714</v>
+        <v>3625.54285714286</v>
       </c>
       <c r="D5" t="n">
-        <v>-2570.9354516885</v>
+        <v>-4149.22267867447</v>
       </c>
       <c r="E5" t="n">
-        <v>12600.6497374028</v>
+        <v>11400.3083929602</v>
       </c>
       <c r="F5" t="n">
-        <v>18.7252257194605</v>
+        <v>13.924323540996</v>
       </c>
       <c r="G5" t="n">
-        <v>-20.5251789172421</v>
+        <v>-25.1256291923018</v>
       </c>
       <c r="H5" t="n">
-        <v>77.3603139975475</v>
+        <v>73.3403747406064</v>
       </c>
     </row>
     <row r="6">
@@ -544,22 +544,22 @@
         <v>473</v>
       </c>
       <c r="C6" t="n">
-        <v>4368.97040169133</v>
+        <v>3901.41014799154</v>
       </c>
       <c r="D6" t="n">
-        <v>2604.28574920508</v>
+        <v>2117.62912208941</v>
       </c>
       <c r="E6" t="n">
-        <v>6133.65505417759</v>
+        <v>5685.19117389367</v>
       </c>
       <c r="F6" t="n">
-        <v>36.0744546211988</v>
+        <v>32.5755195055895</v>
       </c>
       <c r="G6" t="n">
-        <v>22.5295297195276</v>
+        <v>18.9339618162075</v>
       </c>
       <c r="H6" t="n">
-        <v>51.1166919749122</v>
+        <v>47.7817446234417</v>
       </c>
     </row>
     <row r="7">
@@ -570,22 +570,22 @@
         <v>276</v>
       </c>
       <c r="C7" t="n">
-        <v>3714.30434782609</v>
+        <v>3725.05072463768</v>
       </c>
       <c r="D7" t="n">
-        <v>1345.42820276615</v>
+        <v>1326.91865787289</v>
       </c>
       <c r="E7" t="n">
-        <v>6083.18049288603</v>
+        <v>6123.18279140247</v>
       </c>
       <c r="F7" t="n">
-        <v>30.2392039464288</v>
+        <v>27.4953899171181</v>
       </c>
       <c r="G7" t="n">
-        <v>13.1024677211094</v>
+        <v>9.87861037646889</v>
       </c>
       <c r="H7" t="n">
-        <v>49.9724151591934</v>
+        <v>47.9366584126286</v>
       </c>
     </row>
     <row r="8">
@@ -596,22 +596,22 @@
         <v>170</v>
       </c>
       <c r="C8" t="n">
-        <v>5636.87647058823</v>
+        <v>6000.05294117647</v>
       </c>
       <c r="D8" t="n">
-        <v>2389.91143344297</v>
+        <v>2802.2477047623</v>
       </c>
       <c r="E8" t="n">
-        <v>8883.8415077335</v>
+        <v>9197.85817759064</v>
       </c>
       <c r="F8" t="n">
-        <v>44.4752537032238</v>
+        <v>39.3509596377869</v>
       </c>
       <c r="G8" t="n">
-        <v>20.8971405614164</v>
+        <v>17.2298193799924</v>
       </c>
       <c r="H8" t="n">
-        <v>72.651717283646</v>
+        <v>65.6463351617711</v>
       </c>
     </row>
     <row r="9">
@@ -622,22 +622,22 @@
         <v>443</v>
       </c>
       <c r="C9" t="n">
-        <v>5023.00902934537</v>
+        <v>5325.15124153499</v>
       </c>
       <c r="D9" t="n">
-        <v>3420.20197853057</v>
+        <v>3724.153396757</v>
       </c>
       <c r="E9" t="n">
-        <v>6625.81608016017</v>
+        <v>6926.14908631298</v>
       </c>
       <c r="F9" t="n">
-        <v>47.0373790485779</v>
+        <v>52.5102947324947</v>
       </c>
       <c r="G9" t="n">
-        <v>31.7626549789574</v>
+        <v>36.5251185089837</v>
       </c>
       <c r="H9" t="n">
-        <v>64.0828415375197</v>
+        <v>70.3671108541237</v>
       </c>
     </row>
     <row r="10">
@@ -648,22 +648,22 @@
         <v>509</v>
       </c>
       <c r="C10" t="n">
-        <v>6747.08251473477</v>
+        <v>6942.6836935167</v>
       </c>
       <c r="D10" t="n">
-        <v>4998.78019797953</v>
+        <v>5217.34329081175</v>
       </c>
       <c r="E10" t="n">
-        <v>8495.38483149002</v>
+        <v>8668.02409622165</v>
       </c>
       <c r="F10" t="n">
-        <v>58.9136515224582</v>
+        <v>59.9030515466241</v>
       </c>
       <c r="G10" t="n">
-        <v>42.1912411331678</v>
+        <v>43.1983816090779</v>
       </c>
       <c r="H10" t="n">
-        <v>77.602702099986</v>
+        <v>78.5563887427439</v>
       </c>
     </row>
     <row r="11">
@@ -674,22 +674,22 @@
         <v>472</v>
       </c>
       <c r="C11" t="n">
-        <v>9181.90677966102</v>
+        <v>9346.73093220339</v>
       </c>
       <c r="D11" t="n">
-        <v>7128.58815168403</v>
+        <v>7304.51487473163</v>
       </c>
       <c r="E11" t="n">
-        <v>11235.225407638</v>
+        <v>11388.9469896752</v>
       </c>
       <c r="F11" t="n">
-        <v>84.4321060386515</v>
+        <v>81.0533294440124</v>
       </c>
       <c r="G11" t="n">
-        <v>63.2557739018655</v>
+        <v>60.4074873828573</v>
       </c>
       <c r="H11" t="n">
-        <v>108.355275436073</v>
+        <v>104.356471369212</v>
       </c>
     </row>
     <row r="12">
@@ -700,22 +700,22 @@
         <v>648</v>
       </c>
       <c r="C12" t="n">
-        <v>3494.97530864198</v>
+        <v>3878.97530864198</v>
       </c>
       <c r="D12" t="n">
-        <v>2205.86991107789</v>
+        <v>2603.83404312504</v>
       </c>
       <c r="E12" t="n">
-        <v>4784.08070620606</v>
+        <v>5154.11657415891</v>
       </c>
       <c r="F12" t="n">
-        <v>37.0467467969739</v>
+        <v>39.8773166230098</v>
       </c>
       <c r="G12" t="n">
-        <v>24.8773922406321</v>
+        <v>27.4580370845045</v>
       </c>
       <c r="H12" t="n">
-        <v>50.4020100887623</v>
+        <v>53.5067081935502</v>
       </c>
     </row>
     <row r="13">
@@ -726,22 +726,22 @@
         <v>297</v>
       </c>
       <c r="C13" t="n">
-        <v>8624.51515151515</v>
+        <v>8798.75420875421</v>
       </c>
       <c r="D13" t="n">
-        <v>6077.92192409715</v>
+        <v>6254.65384865191</v>
       </c>
       <c r="E13" t="n">
-        <v>11171.1083789332</v>
+        <v>11342.8545688565</v>
       </c>
       <c r="F13" t="n">
-        <v>84.7282247564084</v>
+        <v>85.7811916924413</v>
       </c>
       <c r="G13" t="n">
-        <v>57.3436737872667</v>
+        <v>58.2166269370133</v>
       </c>
       <c r="H13" t="n">
-        <v>116.87886268495</v>
+        <v>118.148066071488</v>
       </c>
     </row>
     <row r="14">
@@ -752,22 +752,22 @@
         <v>203</v>
       </c>
       <c r="C14" t="n">
-        <v>4979.50246305419</v>
+        <v>4496.8275862069</v>
       </c>
       <c r="D14" t="n">
-        <v>2056.40149767035</v>
+        <v>1555.24807449396</v>
       </c>
       <c r="E14" t="n">
-        <v>7902.60342843803</v>
+        <v>7438.40709791983</v>
       </c>
       <c r="F14" t="n">
-        <v>36.9321001411575</v>
+        <v>37.2953957290218</v>
       </c>
       <c r="G14" t="n">
-        <v>15.9861997348303</v>
+        <v>16.3768753089616</v>
       </c>
       <c r="H14" t="n">
-        <v>61.6606121412331</v>
+        <v>61.9739801257333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dopo aver sistemato i siti infetti e il numero di infezioni
</commit_message>
<xml_diff>
--- a/output/risultati.xlsx
+++ b/output/risultati.xlsx
@@ -437,25 +437,25 @@
         <v>8</v>
       </c>
       <c r="B2" t="n">
-        <v>1276</v>
+        <v>1255</v>
       </c>
       <c r="C2" t="n">
-        <v>5370.7578369906</v>
+        <v>5247.01035856574</v>
       </c>
       <c r="D2" t="n">
-        <v>4406.27064705801</v>
+        <v>4259.68905145549</v>
       </c>
       <c r="E2" t="n">
-        <v>6335.24502692318</v>
+        <v>6234.33166567599</v>
       </c>
       <c r="F2" t="n">
-        <v>54.9352742510459</v>
+        <v>53.7238678487814</v>
       </c>
       <c r="G2" t="n">
-        <v>44.366122408994</v>
+        <v>43.3349333927245</v>
       </c>
       <c r="H2" t="n">
-        <v>66.2782016077152</v>
+        <v>64.865793613918</v>
       </c>
     </row>
     <row r="3">
@@ -463,25 +463,25 @@
         <v>9</v>
       </c>
       <c r="B3" t="n">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C3" t="n">
-        <v>5594.49107142857</v>
+        <v>4768.32075471698</v>
       </c>
       <c r="D3" t="n">
-        <v>2048.17652841249</v>
+        <v>1246.6639642203</v>
       </c>
       <c r="E3" t="n">
-        <v>9140.80561444465</v>
+        <v>8289.97754521366</v>
       </c>
       <c r="F3" t="n">
-        <v>41.7779488428836</v>
+        <v>29.9533838592261</v>
       </c>
       <c r="G3" t="n">
-        <v>17.5742847037206</v>
+        <v>6.79666344515095</v>
       </c>
       <c r="H3" t="n">
-        <v>70.9641426162912</v>
+        <v>58.1311759345058</v>
       </c>
     </row>
     <row r="4">
@@ -489,25 +489,25 @@
         <v>10</v>
       </c>
       <c r="B4" t="n">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C4" t="n">
-        <v>5404.29166666667</v>
+        <v>5083.29716981132</v>
       </c>
       <c r="D4" t="n">
-        <v>2433.6978193102</v>
+        <v>1925.62395561542</v>
       </c>
       <c r="E4" t="n">
-        <v>8374.88551402313</v>
+        <v>8240.97038400722</v>
       </c>
       <c r="F4" t="n">
-        <v>44.0519680370241</v>
+        <v>37.5309408963742</v>
       </c>
       <c r="G4" t="n">
-        <v>22.2195148503187</v>
+        <v>15.673427141843</v>
       </c>
       <c r="H4" t="n">
-        <v>69.7844204401677</v>
+        <v>63.5186245553872</v>
       </c>
     </row>
     <row r="5">
@@ -515,25 +515,25 @@
         <v>11</v>
       </c>
       <c r="B5" t="n">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="C5" t="n">
-        <v>2084.57142857143</v>
+        <v>-8218</v>
       </c>
       <c r="D5" t="n">
-        <v>-6227.67295639075</v>
+        <v>-67012.5146420991</v>
       </c>
       <c r="E5" t="n">
-        <v>10396.8158135336</v>
+        <v>50576.5146420991</v>
       </c>
       <c r="F5" t="n">
-        <v>32.4897394714093</v>
+        <v>-66.1499228684452</v>
       </c>
       <c r="G5" t="n">
-        <v>-10.2161016463173</v>
+        <v>-98.2917231587202</v>
       </c>
       <c r="H5" t="n">
-        <v>95.5086756876372</v>
+        <v>570.750603253392</v>
       </c>
     </row>
     <row r="6">
@@ -541,25 +541,25 @@
         <v>12</v>
       </c>
       <c r="B6" t="n">
-        <v>473</v>
+        <v>463</v>
       </c>
       <c r="C6" t="n">
-        <v>4412.15010570825</v>
+        <v>4223.86177105832</v>
       </c>
       <c r="D6" t="n">
-        <v>2649.70914682941</v>
+        <v>2385.15949751633</v>
       </c>
       <c r="E6" t="n">
-        <v>6174.59106458708</v>
+        <v>6062.5640446003</v>
       </c>
       <c r="F6" t="n">
-        <v>35.1779794412802</v>
+        <v>36.7560429998814</v>
       </c>
       <c r="G6" t="n">
-        <v>21.5486214592733</v>
+        <v>22.5634156306051</v>
       </c>
       <c r="H6" t="n">
-        <v>50.3356097868197</v>
+        <v>52.5921515874865</v>
       </c>
     </row>
     <row r="7">
@@ -567,25 +567,25 @@
         <v>13</v>
       </c>
       <c r="B7" t="n">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="C7" t="n">
-        <v>3874.72101449275</v>
+        <v>3486.8962962963</v>
       </c>
       <c r="D7" t="n">
-        <v>1485.80467829147</v>
+        <v>1130.77731253732</v>
       </c>
       <c r="E7" t="n">
-        <v>6263.63735069404</v>
+        <v>5843.01528005527</v>
       </c>
       <c r="F7" t="n">
-        <v>29.5365033258523</v>
+        <v>28.7015248956852</v>
       </c>
       <c r="G7" t="n">
-        <v>11.9296916549961</v>
+        <v>12.1684636931031</v>
       </c>
       <c r="H7" t="n">
-        <v>49.9129091287868</v>
+        <v>47.6714752534599</v>
       </c>
     </row>
     <row r="8">
@@ -593,25 +593,25 @@
         <v>14</v>
       </c>
       <c r="B8" t="n">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C8" t="n">
-        <v>5594.59411764706</v>
+        <v>5303.29696969697</v>
       </c>
       <c r="D8" t="n">
-        <v>2311.11005378345</v>
+        <v>1875.37084991641</v>
       </c>
       <c r="E8" t="n">
-        <v>8878.07818151066</v>
+        <v>8731.22308947753</v>
       </c>
       <c r="F8" t="n">
-        <v>43.8149137118951</v>
+        <v>38.9557843140747</v>
       </c>
       <c r="G8" t="n">
-        <v>20.6764205350851</v>
+        <v>14.9414938196058</v>
       </c>
       <c r="H8" t="n">
-        <v>71.3899808616432</v>
+        <v>67.9872894695763</v>
       </c>
     </row>
     <row r="9">
@@ -619,25 +619,25 @@
         <v>15</v>
       </c>
       <c r="B9" t="n">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="C9" t="n">
-        <v>5126.51467268623</v>
+        <v>5005.44827586207</v>
       </c>
       <c r="D9" t="n">
-        <v>3497.68268254784</v>
+        <v>3324.84368519627</v>
       </c>
       <c r="E9" t="n">
-        <v>6755.34666282462</v>
+        <v>6686.05286652787</v>
       </c>
       <c r="F9" t="n">
-        <v>51.1498522568361</v>
+        <v>39.6853044517943</v>
       </c>
       <c r="G9" t="n">
-        <v>35.7760351066129</v>
+        <v>25.2680763592285</v>
       </c>
       <c r="H9" t="n">
-        <v>68.2644350258439</v>
+        <v>55.7618257331291</v>
       </c>
     </row>
     <row r="10">
@@ -645,25 +645,25 @@
         <v>16</v>
       </c>
       <c r="B10" t="n">
-        <v>509</v>
+        <v>501</v>
       </c>
       <c r="C10" t="n">
-        <v>6871.64440078585</v>
+        <v>6611.32734530938</v>
       </c>
       <c r="D10" t="n">
-        <v>5128.64355070785</v>
+        <v>4807.64893496511</v>
       </c>
       <c r="E10" t="n">
-        <v>8614.64525086386</v>
+        <v>8415.00575565366</v>
       </c>
       <c r="F10" t="n">
-        <v>60.4708833121729</v>
+        <v>61.8168318575774</v>
       </c>
       <c r="G10" t="n">
-        <v>43.9272484646582</v>
+        <v>44.7625769896183</v>
       </c>
       <c r="H10" t="n">
-        <v>78.9161167581984</v>
+        <v>80.8802220638922</v>
       </c>
     </row>
     <row r="11">
@@ -671,25 +671,25 @@
         <v>17</v>
       </c>
       <c r="B11" t="n">
-        <v>472</v>
+        <v>461</v>
       </c>
       <c r="C11" t="n">
-        <v>9263.2436440678</v>
+        <v>9293.39913232104</v>
       </c>
       <c r="D11" t="n">
-        <v>7243.78812070674</v>
+        <v>7228.49207611551</v>
       </c>
       <c r="E11" t="n">
-        <v>11282.6991674289</v>
+        <v>11358.3061885266</v>
       </c>
       <c r="F11" t="n">
-        <v>79.7843417643768</v>
+        <v>77.5932530158467</v>
       </c>
       <c r="G11" t="n">
-        <v>59.1117177860333</v>
+        <v>57.3205814731995</v>
       </c>
       <c r="H11" t="n">
-        <v>103.14286083641</v>
+        <v>100.47830500883</v>
       </c>
     </row>
     <row r="12">
@@ -697,25 +697,25 @@
         <v>18</v>
       </c>
       <c r="B12" t="n">
-        <v>648</v>
+        <v>631</v>
       </c>
       <c r="C12" t="n">
-        <v>3554.3950617284</v>
+        <v>3567.27733755943</v>
       </c>
       <c r="D12" t="n">
-        <v>2249.3327295354</v>
+        <v>2278.17299178467</v>
       </c>
       <c r="E12" t="n">
-        <v>4859.45739392139</v>
+        <v>4856.38168333419</v>
       </c>
       <c r="F12" t="n">
-        <v>39.4231686516458</v>
+        <v>33.720617903291</v>
       </c>
       <c r="G12" t="n">
-        <v>27.1380627871634</v>
+        <v>21.8854097640282</v>
       </c>
       <c r="H12" t="n">
-        <v>52.8953606081525</v>
+        <v>46.7050378470745</v>
       </c>
     </row>
     <row r="13">
@@ -723,25 +723,25 @@
         <v>19</v>
       </c>
       <c r="B13" t="n">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="C13" t="n">
-        <v>9064.32996632997</v>
+        <v>8897.52249134948</v>
       </c>
       <c r="D13" t="n">
-        <v>6536.33248077025</v>
+        <v>6486.7576265608</v>
       </c>
       <c r="E13" t="n">
-        <v>11592.3274518897</v>
+        <v>11308.2873561382</v>
       </c>
       <c r="F13" t="n">
-        <v>82.2022066425796</v>
+        <v>86.3386600004225</v>
       </c>
       <c r="G13" t="n">
-        <v>54.7574422702036</v>
+        <v>59.7818640955245</v>
       </c>
       <c r="H13" t="n">
-        <v>114.514039637996</v>
+        <v>117.309369916943</v>
       </c>
     </row>
     <row r="14">
@@ -752,22 +752,22 @@
         <v>203</v>
       </c>
       <c r="C14" t="n">
-        <v>4994.43842364532</v>
+        <v>4325.71428571429</v>
       </c>
       <c r="D14" t="n">
-        <v>2043.89535200973</v>
+        <v>1267.34382334928</v>
       </c>
       <c r="E14" t="n">
-        <v>7944.98149528091</v>
+        <v>7384.08474807929</v>
       </c>
       <c r="F14" t="n">
-        <v>46.2449717627781</v>
+        <v>37.9133889131261</v>
       </c>
       <c r="G14" t="n">
-        <v>24.139130264227</v>
+        <v>16.532889283864</v>
       </c>
       <c r="H14" t="n">
-        <v>72.2872692951273</v>
+        <v>63.2166074177725</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lavorato alle procedure invasive
</commit_message>
<xml_diff>
--- a/output/risultati.xlsx
+++ b/output/risultati.xlsx
@@ -440,22 +440,22 @@
         <v>1255</v>
       </c>
       <c r="C2" t="n">
-        <v>5247.01035856574</v>
+        <v>5098.05816733068</v>
       </c>
       <c r="D2" t="n">
-        <v>4259.68905145549</v>
+        <v>4123.86856243153</v>
       </c>
       <c r="E2" t="n">
-        <v>6234.33166567599</v>
+        <v>6072.24777222983</v>
       </c>
       <c r="F2" t="n">
-        <v>53.7238678487814</v>
+        <v>51.6894267758399</v>
       </c>
       <c r="G2" t="n">
-        <v>43.3349333927245</v>
+        <v>41.5552281803797</v>
       </c>
       <c r="H2" t="n">
-        <v>64.865793613918</v>
+        <v>62.5491512490258</v>
       </c>
     </row>
     <row r="3">
@@ -466,22 +466,22 @@
         <v>106</v>
       </c>
       <c r="C3" t="n">
-        <v>4768.32075471698</v>
+        <v>5023.22641509434</v>
       </c>
       <c r="D3" t="n">
-        <v>1246.6639642203</v>
+        <v>1509.12645666637</v>
       </c>
       <c r="E3" t="n">
-        <v>8289.97754521366</v>
+        <v>8537.32637352231</v>
       </c>
       <c r="F3" t="n">
-        <v>29.9533838592261</v>
+        <v>18.2657166607197</v>
       </c>
       <c r="G3" t="n">
-        <v>6.79666344515095</v>
+        <v>-2.06951669756918</v>
       </c>
       <c r="H3" t="n">
-        <v>58.1311759345058</v>
+        <v>42.8235546850043</v>
       </c>
     </row>
     <row r="4">
@@ -492,22 +492,22 @@
         <v>212</v>
       </c>
       <c r="C4" t="n">
-        <v>5083.29716981132</v>
+        <v>5290.92452830189</v>
       </c>
       <c r="D4" t="n">
-        <v>1925.62395561542</v>
+        <v>2106.17220545964</v>
       </c>
       <c r="E4" t="n">
-        <v>8240.97038400722</v>
+        <v>8475.67685114414</v>
       </c>
       <c r="F4" t="n">
-        <v>37.5309408963742</v>
+        <v>43.8919402104736</v>
       </c>
       <c r="G4" t="n">
-        <v>15.673427141843</v>
+        <v>21.831791565683</v>
       </c>
       <c r="H4" t="n">
-        <v>63.5186245553872</v>
+        <v>69.9465319474671</v>
       </c>
     </row>
     <row r="5">
@@ -544,22 +544,22 @@
         <v>463</v>
       </c>
       <c r="C6" t="n">
-        <v>4223.86177105832</v>
+        <v>4083.64362850972</v>
       </c>
       <c r="D6" t="n">
-        <v>2385.15949751633</v>
+        <v>2255.88821825647</v>
       </c>
       <c r="E6" t="n">
-        <v>6062.5640446003</v>
+        <v>5911.39903876296</v>
       </c>
       <c r="F6" t="n">
-        <v>36.7560429998814</v>
+        <v>33.6200540541274</v>
       </c>
       <c r="G6" t="n">
-        <v>22.5634156306051</v>
+        <v>19.7635817955482</v>
       </c>
       <c r="H6" t="n">
-        <v>52.5921515874865</v>
+        <v>49.0797000035249</v>
       </c>
     </row>
     <row r="7">
@@ -570,22 +570,22 @@
         <v>270</v>
       </c>
       <c r="C7" t="n">
-        <v>3486.8962962963</v>
+        <v>3312.65555555556</v>
       </c>
       <c r="D7" t="n">
-        <v>1130.77731253732</v>
+        <v>932.718430670331</v>
       </c>
       <c r="E7" t="n">
-        <v>5843.01528005527</v>
+        <v>5692.59268044078</v>
       </c>
       <c r="F7" t="n">
-        <v>28.7015248956852</v>
+        <v>31.6257364882576</v>
       </c>
       <c r="G7" t="n">
-        <v>12.1684636931031</v>
+        <v>13.5393365663865</v>
       </c>
       <c r="H7" t="n">
-        <v>47.6714752534599</v>
+        <v>52.5932335877803</v>
       </c>
     </row>
     <row r="8">
@@ -596,22 +596,22 @@
         <v>165</v>
       </c>
       <c r="C8" t="n">
-        <v>5303.29696969697</v>
+        <v>5007.59393939394</v>
       </c>
       <c r="D8" t="n">
-        <v>1875.37084991641</v>
+        <v>1581.96456750593</v>
       </c>
       <c r="E8" t="n">
-        <v>8731.22308947753</v>
+        <v>8433.22331128194</v>
       </c>
       <c r="F8" t="n">
-        <v>38.9557843140747</v>
+        <v>47.1126719946612</v>
       </c>
       <c r="G8" t="n">
-        <v>14.9414938196058</v>
+        <v>23.3871149009479</v>
       </c>
       <c r="H8" t="n">
-        <v>67.9872894695763</v>
+        <v>75.4003104682571</v>
       </c>
     </row>
     <row r="9">
@@ -622,22 +622,22 @@
         <v>435</v>
       </c>
       <c r="C9" t="n">
-        <v>5005.44827586207</v>
+        <v>4899.42068965517</v>
       </c>
       <c r="D9" t="n">
-        <v>3324.84368519627</v>
+        <v>3205.6369830654</v>
       </c>
       <c r="E9" t="n">
-        <v>6686.05286652787</v>
+        <v>6593.20439624494</v>
       </c>
       <c r="F9" t="n">
-        <v>39.6853044517943</v>
+        <v>45.0694985610431</v>
       </c>
       <c r="G9" t="n">
-        <v>25.2680763592285</v>
+        <v>29.2843603695571</v>
       </c>
       <c r="H9" t="n">
-        <v>55.7618257331291</v>
+        <v>62.7819432497114</v>
       </c>
     </row>
     <row r="10">
@@ -648,22 +648,22 @@
         <v>501</v>
       </c>
       <c r="C10" t="n">
-        <v>6611.32734530938</v>
+        <v>6988.46906187625</v>
       </c>
       <c r="D10" t="n">
-        <v>4807.64893496511</v>
+        <v>5178.68819894672</v>
       </c>
       <c r="E10" t="n">
-        <v>8415.00575565366</v>
+        <v>8798.24992480577</v>
       </c>
       <c r="F10" t="n">
-        <v>61.8168318575774</v>
+        <v>55.9781095189289</v>
       </c>
       <c r="G10" t="n">
-        <v>44.7625769896183</v>
+        <v>38.8006962675155</v>
       </c>
       <c r="H10" t="n">
-        <v>80.8802220638922</v>
+        <v>75.2813300173114</v>
       </c>
     </row>
     <row r="11">
@@ -674,22 +674,22 @@
         <v>461</v>
       </c>
       <c r="C11" t="n">
-        <v>9293.39913232104</v>
+        <v>9002.45986984816</v>
       </c>
       <c r="D11" t="n">
-        <v>7228.49207611551</v>
+        <v>6915.00953084802</v>
       </c>
       <c r="E11" t="n">
-        <v>11358.3061885266</v>
+        <v>11089.9102088483</v>
       </c>
       <c r="F11" t="n">
-        <v>77.5932530158467</v>
+        <v>76.677871922248</v>
       </c>
       <c r="G11" t="n">
-        <v>57.3205814731995</v>
+        <v>56.233875515086</v>
       </c>
       <c r="H11" t="n">
-        <v>100.47830500883</v>
+        <v>99.7970691315284</v>
       </c>
     </row>
     <row r="12">
@@ -700,22 +700,22 @@
         <v>631</v>
       </c>
       <c r="C12" t="n">
-        <v>3567.27733755943</v>
+        <v>3738.33122028526</v>
       </c>
       <c r="D12" t="n">
-        <v>2278.17299178467</v>
+        <v>2465.05451641801</v>
       </c>
       <c r="E12" t="n">
-        <v>4856.38168333419</v>
+        <v>5011.60792415251</v>
       </c>
       <c r="F12" t="n">
-        <v>33.720617903291</v>
+        <v>35.8629493181722</v>
       </c>
       <c r="G12" t="n">
-        <v>21.8854097640282</v>
+        <v>24.1772431550934</v>
       </c>
       <c r="H12" t="n">
-        <v>46.7050378470745</v>
+        <v>48.6483394898521</v>
       </c>
     </row>
     <row r="13">
@@ -726,22 +726,22 @@
         <v>289</v>
       </c>
       <c r="C13" t="n">
-        <v>8897.52249134948</v>
+        <v>8334.723183391</v>
       </c>
       <c r="D13" t="n">
-        <v>6486.7576265608</v>
+        <v>5856.25594222926</v>
       </c>
       <c r="E13" t="n">
-        <v>11308.2873561382</v>
+        <v>10813.1904245527</v>
       </c>
       <c r="F13" t="n">
-        <v>86.3386600004225</v>
+        <v>80.199220189839</v>
       </c>
       <c r="G13" t="n">
-        <v>59.7818640955245</v>
+        <v>54.6165469692269</v>
       </c>
       <c r="H13" t="n">
-        <v>117.309369916943</v>
+        <v>110.014772632899</v>
       </c>
     </row>
     <row r="14">
@@ -752,22 +752,22 @@
         <v>203</v>
       </c>
       <c r="C14" t="n">
-        <v>4325.71428571429</v>
+        <v>4220.30049261084</v>
       </c>
       <c r="D14" t="n">
-        <v>1267.34382334928</v>
+        <v>1143.90518873948</v>
       </c>
       <c r="E14" t="n">
-        <v>7384.08474807929</v>
+        <v>7296.6957964822</v>
       </c>
       <c r="F14" t="n">
-        <v>37.9133889131261</v>
+        <v>30.0845744337273</v>
       </c>
       <c r="G14" t="n">
-        <v>16.532889283864</v>
+        <v>9.10590365598292</v>
       </c>
       <c r="H14" t="n">
-        <v>63.2166074177725</v>
+        <v>55.0969831931365</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
forse non l'avevo fatto prima
</commit_message>
<xml_diff>
--- a/output/risultati.xlsx
+++ b/output/risultati.xlsx
@@ -440,22 +440,22 @@
         <v>1255</v>
       </c>
       <c r="C2" t="n">
-        <v>5098.05816733068</v>
+        <v>5173.30597609562</v>
       </c>
       <c r="D2" t="n">
-        <v>4123.86856243153</v>
+        <v>4183.40169681997</v>
       </c>
       <c r="E2" t="n">
-        <v>6072.24777222983</v>
+        <v>6163.21025537126</v>
       </c>
       <c r="F2" t="n">
-        <v>51.6894267758399</v>
+        <v>49.9077596150444</v>
       </c>
       <c r="G2" t="n">
-        <v>41.5552281803797</v>
+        <v>39.8602772337274</v>
       </c>
       <c r="H2" t="n">
-        <v>62.5491512490258</v>
+        <v>60.6770473881395</v>
       </c>
     </row>
     <row r="3">
@@ -463,25 +463,25 @@
         <v>9</v>
       </c>
       <c r="B3" t="n">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C3" t="n">
-        <v>5023.22641509434</v>
+        <v>4944.17592592593</v>
       </c>
       <c r="D3" t="n">
-        <v>1509.12645666637</v>
+        <v>1238.24599630913</v>
       </c>
       <c r="E3" t="n">
-        <v>8537.32637352231</v>
+        <v>8650.10585554272</v>
       </c>
       <c r="F3" t="n">
-        <v>18.2657166607197</v>
+        <v>32.5396617829015</v>
       </c>
       <c r="G3" t="n">
-        <v>-2.06951669756918</v>
+        <v>7.54678244745857</v>
       </c>
       <c r="H3" t="n">
-        <v>42.8235546850043</v>
+        <v>63.3406555338657</v>
       </c>
     </row>
     <row r="4">
@@ -492,22 +492,22 @@
         <v>212</v>
       </c>
       <c r="C4" t="n">
-        <v>5290.92452830189</v>
+        <v>5352.8679245283</v>
       </c>
       <c r="D4" t="n">
-        <v>2106.17220545964</v>
+        <v>2224.87803180426</v>
       </c>
       <c r="E4" t="n">
-        <v>8475.67685114414</v>
+        <v>8480.85781725235</v>
       </c>
       <c r="F4" t="n">
-        <v>43.8919402104736</v>
+        <v>39.3094744946566</v>
       </c>
       <c r="G4" t="n">
-        <v>21.831791565683</v>
+        <v>17.3977231146548</v>
       </c>
       <c r="H4" t="n">
-        <v>69.9465319474671</v>
+        <v>65.310954668377</v>
       </c>
     </row>
     <row r="5">
@@ -541,25 +541,25 @@
         <v>12</v>
       </c>
       <c r="B6" t="n">
-        <v>463</v>
+        <v>480</v>
       </c>
       <c r="C6" t="n">
-        <v>4083.64362850972</v>
+        <v>4490.13125</v>
       </c>
       <c r="D6" t="n">
-        <v>2255.88821825647</v>
+        <v>2710.58975503441</v>
       </c>
       <c r="E6" t="n">
-        <v>5911.39903876296</v>
+        <v>6269.67274496559</v>
       </c>
       <c r="F6" t="n">
-        <v>33.6200540541274</v>
+        <v>37.0551130862287</v>
       </c>
       <c r="G6" t="n">
-        <v>19.7635817955482</v>
+        <v>22.7415476871315</v>
       </c>
       <c r="H6" t="n">
-        <v>49.0797000035249</v>
+        <v>53.0378618897625</v>
       </c>
     </row>
     <row r="7">
@@ -570,22 +570,22 @@
         <v>270</v>
       </c>
       <c r="C7" t="n">
-        <v>3312.65555555556</v>
+        <v>3091.62592592593</v>
       </c>
       <c r="D7" t="n">
-        <v>932.718430670331</v>
+        <v>695.420024451337</v>
       </c>
       <c r="E7" t="n">
-        <v>5692.59268044078</v>
+        <v>5487.83182740052</v>
       </c>
       <c r="F7" t="n">
-        <v>31.6257364882576</v>
+        <v>27.8254842217933</v>
       </c>
       <c r="G7" t="n">
-        <v>13.5393365663865</v>
+        <v>11.1079252499772</v>
       </c>
       <c r="H7" t="n">
-        <v>52.5932335877803</v>
+        <v>47.0584063177734</v>
       </c>
     </row>
     <row r="8">
@@ -593,25 +593,25 @@
         <v>14</v>
       </c>
       <c r="B8" t="n">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C8" t="n">
-        <v>5007.59393939394</v>
+        <v>5004.52694610778</v>
       </c>
       <c r="D8" t="n">
-        <v>1581.96456750593</v>
+        <v>1771.84582513497</v>
       </c>
       <c r="E8" t="n">
-        <v>8433.22331128194</v>
+        <v>8237.2080670806</v>
       </c>
       <c r="F8" t="n">
-        <v>47.1126719946612</v>
+        <v>29.5130207619676</v>
       </c>
       <c r="G8" t="n">
-        <v>23.3871149009479</v>
+        <v>7.9491671949834</v>
       </c>
       <c r="H8" t="n">
-        <v>75.4003104682571</v>
+        <v>55.3844553204609</v>
       </c>
     </row>
     <row r="9">
@@ -622,22 +622,22 @@
         <v>435</v>
       </c>
       <c r="C9" t="n">
-        <v>4899.42068965517</v>
+        <v>4225.53103448276</v>
       </c>
       <c r="D9" t="n">
-        <v>3205.6369830654</v>
+        <v>2512.28954643103</v>
       </c>
       <c r="E9" t="n">
-        <v>6593.20439624494</v>
+        <v>5938.77252253448</v>
       </c>
       <c r="F9" t="n">
-        <v>45.0694985610431</v>
+        <v>43.477212421635</v>
       </c>
       <c r="G9" t="n">
-        <v>29.2843603695571</v>
+        <v>28.0575735987752</v>
       </c>
       <c r="H9" t="n">
-        <v>62.7819432497114</v>
+        <v>60.7535572146734</v>
       </c>
     </row>
     <row r="10">
@@ -648,22 +648,22 @@
         <v>501</v>
       </c>
       <c r="C10" t="n">
-        <v>6988.46906187625</v>
+        <v>6404.95808383234</v>
       </c>
       <c r="D10" t="n">
-        <v>5178.68819894672</v>
+        <v>4547.11618993366</v>
       </c>
       <c r="E10" t="n">
-        <v>8798.24992480577</v>
+        <v>8262.79997773101</v>
       </c>
       <c r="F10" t="n">
-        <v>55.9781095189289</v>
+        <v>55.8864347601714</v>
       </c>
       <c r="G10" t="n">
-        <v>38.8006962675155</v>
+        <v>39.1337615202656</v>
       </c>
       <c r="H10" t="n">
-        <v>75.2813300173114</v>
+        <v>74.6562464545866</v>
       </c>
     </row>
     <row r="11">
@@ -674,22 +674,22 @@
         <v>461</v>
       </c>
       <c r="C11" t="n">
-        <v>9002.45986984816</v>
+        <v>8924.96095444685</v>
       </c>
       <c r="D11" t="n">
-        <v>6915.00953084802</v>
+        <v>6825.86237875215</v>
       </c>
       <c r="E11" t="n">
-        <v>11089.9102088483</v>
+        <v>11024.0595301416</v>
       </c>
       <c r="F11" t="n">
-        <v>76.677871922248</v>
+        <v>73.9079551834024</v>
       </c>
       <c r="G11" t="n">
-        <v>56.233875515086</v>
+        <v>53.5882163254928</v>
       </c>
       <c r="H11" t="n">
-        <v>99.7970691315284</v>
+        <v>96.915997852189</v>
       </c>
     </row>
     <row r="12">
@@ -700,22 +700,22 @@
         <v>631</v>
       </c>
       <c r="C12" t="n">
-        <v>3738.33122028526</v>
+        <v>3849.92234548336</v>
       </c>
       <c r="D12" t="n">
-        <v>2465.05451641801</v>
+        <v>2597.48356986861</v>
       </c>
       <c r="E12" t="n">
-        <v>5011.60792415251</v>
+        <v>5102.36112109811</v>
       </c>
       <c r="F12" t="n">
-        <v>35.8629493181722</v>
+        <v>38.8878365922042</v>
       </c>
       <c r="G12" t="n">
-        <v>24.1772431550934</v>
+        <v>26.6189019043628</v>
       </c>
       <c r="H12" t="n">
-        <v>48.6483394898521</v>
+        <v>52.3455887165466</v>
       </c>
     </row>
     <row r="13">
@@ -726,22 +726,22 @@
         <v>289</v>
       </c>
       <c r="C13" t="n">
-        <v>8334.723183391</v>
+        <v>8659.11764705882</v>
       </c>
       <c r="D13" t="n">
-        <v>5856.25594222926</v>
+        <v>6201.0046028662</v>
       </c>
       <c r="E13" t="n">
-        <v>10813.1904245527</v>
+        <v>11117.2306912515</v>
       </c>
       <c r="F13" t="n">
-        <v>80.199220189839</v>
+        <v>84.774609426636</v>
       </c>
       <c r="G13" t="n">
-        <v>54.6165469692269</v>
+        <v>58.4640329296849</v>
       </c>
       <c r="H13" t="n">
-        <v>110.014772632899</v>
+        <v>115.453662623338</v>
       </c>
     </row>
     <row r="14">
@@ -752,22 +752,22 @@
         <v>203</v>
       </c>
       <c r="C14" t="n">
-        <v>4220.30049261084</v>
+        <v>4280.10837438424</v>
       </c>
       <c r="D14" t="n">
-        <v>1143.90518873948</v>
+        <v>1228.00040083513</v>
       </c>
       <c r="E14" t="n">
-        <v>7296.6957964822</v>
+        <v>7332.21634793334</v>
       </c>
       <c r="F14" t="n">
-        <v>30.0845744337273</v>
+        <v>39.6894796126501</v>
       </c>
       <c r="G14" t="n">
-        <v>9.10590365598292</v>
+        <v>17.7051091679091</v>
       </c>
       <c r="H14" t="n">
-        <v>55.0969831931365</v>
+        <v>65.7799806006469</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sistemate le procedure invasive
</commit_message>
<xml_diff>
--- a/output/risultati.xlsx
+++ b/output/risultati.xlsx
@@ -440,22 +440,22 @@
         <v>1350</v>
       </c>
       <c r="C2" t="n">
-        <v>5813.06222222222</v>
+        <v>5807.99333333333</v>
       </c>
       <c r="D2" t="n">
-        <v>4865.03219436376</v>
+        <v>4855.67000424764</v>
       </c>
       <c r="E2" t="n">
-        <v>6761.09225008068</v>
+        <v>6760.31666241903</v>
       </c>
       <c r="F2" t="n">
-        <v>55.5459009356584</v>
+        <v>53.9760435303685</v>
       </c>
       <c r="G2" t="n">
-        <v>45.2685916647577</v>
+        <v>43.8447940458174</v>
       </c>
       <c r="H2" t="n">
-        <v>66.550298454881</v>
+        <v>64.8208552734572</v>
       </c>
     </row>
     <row r="3">
@@ -466,22 +466,22 @@
         <v>139</v>
       </c>
       <c r="C3" t="n">
-        <v>7163.94964028777</v>
+        <v>6644.35251798561</v>
       </c>
       <c r="D3" t="n">
-        <v>3661.73651140874</v>
+        <v>3130.31491519274</v>
       </c>
       <c r="E3" t="n">
-        <v>10666.1627691668</v>
+        <v>10158.3901207785</v>
       </c>
       <c r="F3" t="n">
-        <v>48.8296604619294</v>
+        <v>44.6564839335076</v>
       </c>
       <c r="G3" t="n">
-        <v>23.4620529407042</v>
+        <v>19.8770485409426</v>
       </c>
       <c r="H3" t="n">
-        <v>79.4095214328846</v>
+        <v>74.5580042109418</v>
       </c>
     </row>
     <row r="4">
@@ -492,22 +492,22 @@
         <v>261</v>
       </c>
       <c r="C4" t="n">
-        <v>6961.80842911877</v>
+        <v>6970.97318007663</v>
       </c>
       <c r="D4" t="n">
-        <v>4218.81038829578</v>
+        <v>4214.90984201603</v>
       </c>
       <c r="E4" t="n">
-        <v>9704.80646994177</v>
+        <v>9727.03651813723</v>
       </c>
       <c r="F4" t="n">
-        <v>66.9808285411527</v>
+        <v>58.2167158235049</v>
       </c>
       <c r="G4" t="n">
-        <v>40.341880927658</v>
+        <v>33.0964458856711</v>
       </c>
       <c r="H4" t="n">
-        <v>98.6762391667138</v>
+        <v>88.0781188363096</v>
       </c>
     </row>
     <row r="5">
@@ -518,22 +518,22 @@
         <v>35</v>
       </c>
       <c r="C5" t="n">
-        <v>5812.71428571429</v>
+        <v>6619.54285714286</v>
       </c>
       <c r="D5" t="n">
-        <v>-1414.1352472354</v>
+        <v>-417.086371763283</v>
       </c>
       <c r="E5" t="n">
-        <v>13039.563818664</v>
+        <v>13656.172086049</v>
       </c>
       <c r="F5" t="n">
-        <v>53.6913057921562</v>
+        <v>56.1391912395674</v>
       </c>
       <c r="G5" t="n">
-        <v>-1.72314443495992</v>
+        <v>3.55265678560925</v>
       </c>
       <c r="H5" t="n">
-        <v>140.351783136423</v>
+        <v>135.430435082127</v>
       </c>
     </row>
     <row r="6">
@@ -544,22 +544,22 @@
         <v>510</v>
       </c>
       <c r="C6" t="n">
-        <v>4704.07254901961</v>
+        <v>5020.51176470588</v>
       </c>
       <c r="D6" t="n">
-        <v>2954.8283999128</v>
+        <v>3295.51733422747</v>
       </c>
       <c r="E6" t="n">
-        <v>6453.31669812642</v>
+        <v>6745.50619518429</v>
       </c>
       <c r="F6" t="n">
-        <v>38.5442042766873</v>
+        <v>44.7355385388438</v>
       </c>
       <c r="G6" t="n">
-        <v>24.0547889416789</v>
+        <v>29.9022197539786</v>
       </c>
       <c r="H6" t="n">
-        <v>54.7259618303349</v>
+        <v>61.262649366602</v>
       </c>
     </row>
     <row r="7">
@@ -570,22 +570,22 @@
         <v>287</v>
       </c>
       <c r="C7" t="n">
-        <v>3318.10104529617</v>
+        <v>3619.74216027875</v>
       </c>
       <c r="D7" t="n">
-        <v>806.884317947733</v>
+        <v>1140.7151108601</v>
       </c>
       <c r="E7" t="n">
-        <v>5829.3177726446</v>
+        <v>6098.76920969739</v>
       </c>
       <c r="F7" t="n">
-        <v>27.7276273923899</v>
+        <v>19.8694162093934</v>
       </c>
       <c r="G7" t="n">
-        <v>10.8662674835068</v>
+        <v>2.40293877720188</v>
       </c>
       <c r="H7" t="n">
-        <v>47.1533873160854</v>
+        <v>40.315083863391</v>
       </c>
     </row>
     <row r="8">
@@ -596,22 +596,22 @@
         <v>184</v>
       </c>
       <c r="C8" t="n">
-        <v>6229.82608695652</v>
+        <v>6097.0652173913</v>
       </c>
       <c r="D8" t="n">
-        <v>3251.70509578649</v>
+        <v>3063.92640999149</v>
       </c>
       <c r="E8" t="n">
-        <v>9207.94707812656</v>
+        <v>9130.20402479112</v>
       </c>
       <c r="F8" t="n">
-        <v>47.8107071026915</v>
+        <v>35.5654053995403</v>
       </c>
       <c r="G8" t="n">
-        <v>23.7498354063453</v>
+        <v>13.3427839659655</v>
       </c>
       <c r="H8" t="n">
-        <v>76.5497712579372</v>
+        <v>62.1451185340588</v>
       </c>
     </row>
     <row r="9">
@@ -622,22 +622,22 @@
         <v>473</v>
       </c>
       <c r="C9" t="n">
-        <v>5857.81606765328</v>
+        <v>6088.94926004228</v>
       </c>
       <c r="D9" t="n">
-        <v>4241.13842422649</v>
+        <v>4492.15432076563</v>
       </c>
       <c r="E9" t="n">
-        <v>7474.49371108006</v>
+        <v>7685.74419931894</v>
       </c>
       <c r="F9" t="n">
-        <v>54.1395423190276</v>
+        <v>54.0900366192973</v>
       </c>
       <c r="G9" t="n">
-        <v>38.5706200315785</v>
+        <v>38.3054790735635</v>
       </c>
       <c r="H9" t="n">
-        <v>71.4576906771792</v>
+        <v>71.6760575530584</v>
       </c>
     </row>
     <row r="10">
@@ -648,22 +648,22 @@
         <v>543</v>
       </c>
       <c r="C10" t="n">
-        <v>7595.79189686924</v>
+        <v>7636.37384898711</v>
       </c>
       <c r="D10" t="n">
-        <v>5859.87431695783</v>
+        <v>5876.46864893458</v>
       </c>
       <c r="E10" t="n">
-        <v>9331.70947678066</v>
+        <v>9396.27904903964</v>
       </c>
       <c r="F10" t="n">
-        <v>61.6515614377799</v>
+        <v>60.4975508251942</v>
       </c>
       <c r="G10" t="n">
-        <v>45.1272559603083</v>
+        <v>43.8285646268481</v>
       </c>
       <c r="H10" t="n">
-        <v>80.0573375577302</v>
+        <v>79.098386246965</v>
       </c>
     </row>
     <row r="11">
@@ -674,22 +674,22 @@
         <v>509</v>
       </c>
       <c r="C11" t="n">
-        <v>10112.0432220039</v>
+        <v>9950.73280943026</v>
       </c>
       <c r="D11" t="n">
-        <v>8101.47413503325</v>
+        <v>7921.78186846451</v>
       </c>
       <c r="E11" t="n">
-        <v>12122.6123089746</v>
+        <v>11979.683750396</v>
       </c>
       <c r="F11" t="n">
-        <v>91.9420953271509</v>
+        <v>82.9410667004864</v>
       </c>
       <c r="G11" t="n">
-        <v>70.3431066852557</v>
+        <v>62.3965904229516</v>
       </c>
       <c r="H11" t="n">
-        <v>116.27977013857</v>
+        <v>106.08458464767</v>
       </c>
     </row>
     <row r="12">
@@ -700,22 +700,22 @@
         <v>680</v>
       </c>
       <c r="C12" t="n">
-        <v>4501.90441176471</v>
+        <v>4480.01323529412</v>
       </c>
       <c r="D12" t="n">
-        <v>3255.31231883054</v>
+        <v>3253.60221519012</v>
       </c>
       <c r="E12" t="n">
-        <v>5748.49650469887</v>
+        <v>5706.42425539812</v>
       </c>
       <c r="F12" t="n">
-        <v>46.4901926570979</v>
+        <v>49.7753475721206</v>
       </c>
       <c r="G12" t="n">
-        <v>33.9369515661543</v>
+        <v>36.6815663265411</v>
       </c>
       <c r="H12" t="n">
-        <v>60.2199862979143</v>
+        <v>64.1234830946879</v>
       </c>
     </row>
     <row r="13">
@@ -726,22 +726,22 @@
         <v>328</v>
       </c>
       <c r="C13" t="n">
-        <v>9529.77134146341</v>
+        <v>9557.82317073171</v>
       </c>
       <c r="D13" t="n">
-        <v>7149.09627142381</v>
+        <v>7182.99580392167</v>
       </c>
       <c r="E13" t="n">
-        <v>11910.446411503</v>
+        <v>11932.6505375417</v>
       </c>
       <c r="F13" t="n">
-        <v>91.4532013018841</v>
+        <v>90.8842070539401</v>
       </c>
       <c r="G13" t="n">
-        <v>65.0627731292905</v>
+        <v>64.9825415136985</v>
       </c>
       <c r="H13" t="n">
-        <v>122.062961828644</v>
+        <v>120.852340910181</v>
       </c>
     </row>
     <row r="14">
@@ -752,22 +752,22 @@
         <v>221</v>
       </c>
       <c r="C14" t="n">
-        <v>5722.04977375566</v>
+        <v>5380.85972850679</v>
       </c>
       <c r="D14" t="n">
-        <v>3045.41700719008</v>
+        <v>2663.67094096935</v>
       </c>
       <c r="E14" t="n">
-        <v>8398.68254032123</v>
+        <v>8098.04851604422</v>
       </c>
       <c r="F14" t="n">
-        <v>55.3556206788781</v>
+        <v>36.7634470939795</v>
       </c>
       <c r="G14" t="n">
-        <v>32.7393772633072</v>
+        <v>17.02188460142</v>
       </c>
       <c r="H14" t="n">
-        <v>81.8252381028092</v>
+        <v>59.8354062125637</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corretto data proc invasive, UOC neurochirurgia come reparto di riferimento
</commit_message>
<xml_diff>
--- a/output/risultati.xlsx
+++ b/output/risultati.xlsx
@@ -440,22 +440,22 @@
         <v>1350</v>
       </c>
       <c r="C2" t="n">
-        <v>5807.99333333333</v>
+        <v>5715.21259259259</v>
       </c>
       <c r="D2" t="n">
-        <v>4855.67000424764</v>
+        <v>4755.59365903528</v>
       </c>
       <c r="E2" t="n">
-        <v>6760.31666241903</v>
+        <v>6674.8315261499</v>
       </c>
       <c r="F2" t="n">
-        <v>53.9760435303685</v>
+        <v>58.4736690232438</v>
       </c>
       <c r="G2" t="n">
-        <v>43.8447940458174</v>
+        <v>48.0412061479761</v>
       </c>
       <c r="H2" t="n">
-        <v>64.8208552734572</v>
+        <v>69.6413074923597</v>
       </c>
     </row>
     <row r="3">
@@ -466,22 +466,22 @@
         <v>139</v>
       </c>
       <c r="C3" t="n">
-        <v>6644.35251798561</v>
+        <v>7591.30215827338</v>
       </c>
       <c r="D3" t="n">
-        <v>3130.31491519274</v>
+        <v>4180.26307059955</v>
       </c>
       <c r="E3" t="n">
-        <v>10158.3901207785</v>
+        <v>11002.3412459472</v>
       </c>
       <c r="F3" t="n">
-        <v>44.6564839335076</v>
+        <v>48.9998266489516</v>
       </c>
       <c r="G3" t="n">
-        <v>19.8770485409426</v>
+        <v>22.640584900941</v>
       </c>
       <c r="H3" t="n">
-        <v>74.5580042109418</v>
+        <v>81.0244818984657</v>
       </c>
     </row>
     <row r="4">
@@ -492,22 +492,22 @@
         <v>261</v>
       </c>
       <c r="C4" t="n">
-        <v>6970.97318007663</v>
+        <v>6976.44827586207</v>
       </c>
       <c r="D4" t="n">
-        <v>4214.90984201603</v>
+        <v>4227.32196803053</v>
       </c>
       <c r="E4" t="n">
-        <v>9727.03651813723</v>
+        <v>9725.57458369361</v>
       </c>
       <c r="F4" t="n">
-        <v>58.2167158235049</v>
+        <v>58.9461068505946</v>
       </c>
       <c r="G4" t="n">
-        <v>33.0964458856711</v>
+        <v>34.0551918863844</v>
       </c>
       <c r="H4" t="n">
-        <v>88.0781188363096</v>
+        <v>88.4586827817343</v>
       </c>
     </row>
     <row r="5">
@@ -518,22 +518,22 @@
         <v>35</v>
       </c>
       <c r="C5" t="n">
-        <v>6619.54285714286</v>
+        <v>6559.02857142857</v>
       </c>
       <c r="D5" t="n">
-        <v>-417.086371763283</v>
+        <v>-492.471476130318</v>
       </c>
       <c r="E5" t="n">
-        <v>13656.172086049</v>
+        <v>13610.5286189875</v>
       </c>
       <c r="F5" t="n">
-        <v>56.1391912395674</v>
+        <v>46.298727633075</v>
       </c>
       <c r="G5" t="n">
-        <v>3.55265678560925</v>
+        <v>-4.67402246824763</v>
       </c>
       <c r="H5" t="n">
-        <v>135.430435082127</v>
+        <v>124.527649873062</v>
       </c>
     </row>
     <row r="6">
@@ -544,22 +544,22 @@
         <v>510</v>
       </c>
       <c r="C6" t="n">
-        <v>5020.51176470588</v>
+        <v>4728.76862745098</v>
       </c>
       <c r="D6" t="n">
-        <v>3295.51733422747</v>
+        <v>2969.80577555462</v>
       </c>
       <c r="E6" t="n">
-        <v>6745.50619518429</v>
+        <v>6487.73147934734</v>
       </c>
       <c r="F6" t="n">
-        <v>44.7355385388438</v>
+        <v>41.6683035115908</v>
       </c>
       <c r="G6" t="n">
-        <v>29.9022197539786</v>
+        <v>27.3690084481607</v>
       </c>
       <c r="H6" t="n">
-        <v>61.262649366602</v>
+        <v>57.5729328851664</v>
       </c>
     </row>
     <row r="7">
@@ -570,22 +570,22 @@
         <v>287</v>
       </c>
       <c r="C7" t="n">
-        <v>3619.74216027875</v>
+        <v>4012.29965156794</v>
       </c>
       <c r="D7" t="n">
-        <v>1140.7151108601</v>
+        <v>1549.7222994326</v>
       </c>
       <c r="E7" t="n">
-        <v>6098.76920969739</v>
+        <v>6474.87700370329</v>
       </c>
       <c r="F7" t="n">
-        <v>19.8694162093934</v>
+        <v>23.8659014613487</v>
       </c>
       <c r="G7" t="n">
-        <v>2.40293877720188</v>
+        <v>6.84649947783738</v>
       </c>
       <c r="H7" t="n">
-        <v>40.315083863391</v>
+        <v>43.5962958057882</v>
       </c>
     </row>
     <row r="8">
@@ -596,22 +596,22 @@
         <v>184</v>
       </c>
       <c r="C8" t="n">
-        <v>6097.0652173913</v>
+        <v>5905.4402173913</v>
       </c>
       <c r="D8" t="n">
-        <v>3063.92640999149</v>
+        <v>2889.42549041559</v>
       </c>
       <c r="E8" t="n">
-        <v>9130.20402479112</v>
+        <v>8921.45494436702</v>
       </c>
       <c r="F8" t="n">
-        <v>35.5654053995403</v>
+        <v>44.8845316038222</v>
       </c>
       <c r="G8" t="n">
-        <v>13.3427839659655</v>
+        <v>21.41121023058</v>
       </c>
       <c r="H8" t="n">
-        <v>62.1451185340588</v>
+        <v>72.8961226742783</v>
       </c>
     </row>
     <row r="9">
@@ -622,22 +622,22 @@
         <v>473</v>
       </c>
       <c r="C9" t="n">
-        <v>6088.94926004228</v>
+        <v>5941.61733615222</v>
       </c>
       <c r="D9" t="n">
-        <v>4492.15432076563</v>
+        <v>4306.84686242448</v>
       </c>
       <c r="E9" t="n">
-        <v>7685.74419931894</v>
+        <v>7576.38780987996</v>
       </c>
       <c r="F9" t="n">
-        <v>54.0900366192973</v>
+        <v>54.4490455677735</v>
       </c>
       <c r="G9" t="n">
-        <v>38.3054790735635</v>
+        <v>38.4040986642213</v>
       </c>
       <c r="H9" t="n">
-        <v>71.6760575530584</v>
+        <v>72.3540553135569</v>
       </c>
     </row>
     <row r="10">
@@ -648,22 +648,22 @@
         <v>543</v>
       </c>
       <c r="C10" t="n">
-        <v>7636.37384898711</v>
+        <v>7767.69244935543</v>
       </c>
       <c r="D10" t="n">
-        <v>5876.46864893458</v>
+        <v>6035.88844322261</v>
       </c>
       <c r="E10" t="n">
-        <v>9396.27904903964</v>
+        <v>9499.49645548826</v>
       </c>
       <c r="F10" t="n">
-        <v>60.4975508251942</v>
+        <v>63.5287467489932</v>
       </c>
       <c r="G10" t="n">
-        <v>43.8285646268481</v>
+        <v>46.6978910518555</v>
       </c>
       <c r="H10" t="n">
-        <v>79.098386246965</v>
+        <v>82.2906302302846</v>
       </c>
     </row>
     <row r="11">
@@ -674,22 +674,22 @@
         <v>509</v>
       </c>
       <c r="C11" t="n">
-        <v>9950.73280943026</v>
+        <v>9986.43418467583</v>
       </c>
       <c r="D11" t="n">
-        <v>7921.78186846451</v>
+        <v>7968.512908009</v>
       </c>
       <c r="E11" t="n">
-        <v>11979.683750396</v>
+        <v>12004.3554613427</v>
       </c>
       <c r="F11" t="n">
-        <v>82.9410667004864</v>
+        <v>84.629022437725</v>
       </c>
       <c r="G11" t="n">
-        <v>62.3965904229516</v>
+        <v>63.4141853892643</v>
       </c>
       <c r="H11" t="n">
-        <v>106.08458464767</v>
+        <v>108.598022534642</v>
       </c>
     </row>
     <row r="12">
@@ -700,22 +700,22 @@
         <v>680</v>
       </c>
       <c r="C12" t="n">
-        <v>4480.01323529412</v>
+        <v>4695.12058823529</v>
       </c>
       <c r="D12" t="n">
-        <v>3253.60221519012</v>
+        <v>3482.82323385664</v>
       </c>
       <c r="E12" t="n">
-        <v>5706.42425539812</v>
+        <v>5907.41794261395</v>
       </c>
       <c r="F12" t="n">
-        <v>49.7753475721206</v>
+        <v>41.2873374027604</v>
       </c>
       <c r="G12" t="n">
-        <v>36.6815663265411</v>
+        <v>29.1788613355816</v>
       </c>
       <c r="H12" t="n">
-        <v>64.1234830946879</v>
+        <v>54.5307916788627</v>
       </c>
     </row>
     <row r="13">
@@ -726,22 +726,22 @@
         <v>328</v>
       </c>
       <c r="C13" t="n">
-        <v>9557.82317073171</v>
+        <v>9635.97256097561</v>
       </c>
       <c r="D13" t="n">
-        <v>7182.99580392167</v>
+        <v>7277.18306734735</v>
       </c>
       <c r="E13" t="n">
-        <v>11932.6505375417</v>
+        <v>11994.7620546039</v>
       </c>
       <c r="F13" t="n">
-        <v>90.8842070539401</v>
+        <v>86.141824160658</v>
       </c>
       <c r="G13" t="n">
-        <v>64.9825415136985</v>
+        <v>60.8955424557884</v>
       </c>
       <c r="H13" t="n">
-        <v>120.852340910181</v>
+        <v>115.349525369096</v>
       </c>
     </row>
     <row r="14">
@@ -752,22 +752,22 @@
         <v>221</v>
       </c>
       <c r="C14" t="n">
-        <v>5380.85972850679</v>
+        <v>5363.75113122172</v>
       </c>
       <c r="D14" t="n">
-        <v>2663.67094096935</v>
+        <v>2704.66743607948</v>
       </c>
       <c r="E14" t="n">
-        <v>8098.04851604422</v>
+        <v>8022.83482636396</v>
       </c>
       <c r="F14" t="n">
-        <v>36.7634470939795</v>
+        <v>50.8517269867928</v>
       </c>
       <c r="G14" t="n">
-        <v>17.02188460142</v>
+        <v>29.0932322739088</v>
       </c>
       <c r="H14" t="n">
-        <v>59.8354062125637</v>
+        <v>76.2775873998869</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mancavano i risultati esportati
</commit_message>
<xml_diff>
--- a/output/risultati.xlsx
+++ b/output/risultati.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t xml:space="preserve">Batteri.Siti</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t xml:space="preserve">Wound</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rectal</t>
   </si>
 </sst>
 </file>
@@ -437,25 +440,25 @@
         <v>8</v>
       </c>
       <c r="B2" t="n">
-        <v>1350</v>
+        <v>1212</v>
       </c>
       <c r="C2" t="n">
-        <v>5715.21259259259</v>
+        <v>4864.78300330033</v>
       </c>
       <c r="D2" t="n">
-        <v>4755.59365903528</v>
+        <v>4030.62673192859</v>
       </c>
       <c r="E2" t="n">
-        <v>6674.8315261499</v>
+        <v>5698.93927467208</v>
       </c>
       <c r="F2" t="n">
-        <v>58.4736690232438</v>
+        <v>64.8884217351934</v>
       </c>
       <c r="G2" t="n">
-        <v>48.0412061479761</v>
+        <v>53.9111984327623</v>
       </c>
       <c r="H2" t="n">
-        <v>69.6413074923597</v>
+        <v>76.6485603333175</v>
       </c>
     </row>
     <row r="3">
@@ -463,25 +466,25 @@
         <v>9</v>
       </c>
       <c r="B3" t="n">
-        <v>139</v>
+        <v>93</v>
       </c>
       <c r="C3" t="n">
-        <v>7591.30215827338</v>
+        <v>6124.32258064516</v>
       </c>
       <c r="D3" t="n">
-        <v>4180.26307059955</v>
+        <v>3226.79203284396</v>
       </c>
       <c r="E3" t="n">
-        <v>11002.3412459472</v>
+        <v>9021.85312844636</v>
       </c>
       <c r="F3" t="n">
-        <v>48.9998266489516</v>
+        <v>64.6167943642757</v>
       </c>
       <c r="G3" t="n">
-        <v>22.640584900941</v>
+        <v>36.1918016499488</v>
       </c>
       <c r="H3" t="n">
-        <v>81.0244818984657</v>
+        <v>98.9744511671965</v>
       </c>
     </row>
     <row r="4">
@@ -489,25 +492,25 @@
         <v>10</v>
       </c>
       <c r="B4" t="n">
-        <v>261</v>
+        <v>207</v>
       </c>
       <c r="C4" t="n">
-        <v>6976.44827586207</v>
+        <v>7897.14975845411</v>
       </c>
       <c r="D4" t="n">
-        <v>4227.32196803053</v>
+        <v>5602.10540821417</v>
       </c>
       <c r="E4" t="n">
-        <v>9725.57458369361</v>
+        <v>10192.194108694</v>
       </c>
       <c r="F4" t="n">
-        <v>58.9461068505946</v>
+        <v>96.8953873520834</v>
       </c>
       <c r="G4" t="n">
-        <v>34.0551918863844</v>
+        <v>69.7943364112936</v>
       </c>
       <c r="H4" t="n">
-        <v>88.4586827817343</v>
+        <v>128.322065269713</v>
       </c>
     </row>
     <row r="5">
@@ -515,25 +518,25 @@
         <v>11</v>
       </c>
       <c r="B5" t="n">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C5" t="n">
-        <v>6559.02857142857</v>
+        <v>2461.88888888889</v>
       </c>
       <c r="D5" t="n">
-        <v>-492.471476130318</v>
+        <v>-198.034289005532</v>
       </c>
       <c r="E5" t="n">
-        <v>13610.5286189875</v>
+        <v>5121.81206678331</v>
       </c>
       <c r="F5" t="n">
-        <v>46.298727633075</v>
+        <v>72.3972877312904</v>
       </c>
       <c r="G5" t="n">
-        <v>-4.67402246824763</v>
+        <v>15.4373426626473</v>
       </c>
       <c r="H5" t="n">
-        <v>124.527649873062</v>
+        <v>157.462829025449</v>
       </c>
     </row>
     <row r="6">
@@ -541,25 +544,25 @@
         <v>12</v>
       </c>
       <c r="B6" t="n">
-        <v>510</v>
+        <v>441</v>
       </c>
       <c r="C6" t="n">
-        <v>4728.76862745098</v>
+        <v>5090.07936507936</v>
       </c>
       <c r="D6" t="n">
-        <v>2969.80577555462</v>
+        <v>3754.05071928177</v>
       </c>
       <c r="E6" t="n">
-        <v>6487.73147934734</v>
+        <v>6426.10801087696</v>
       </c>
       <c r="F6" t="n">
-        <v>41.6683035115908</v>
+        <v>65.5078750545022</v>
       </c>
       <c r="G6" t="n">
-        <v>27.3690084481607</v>
+        <v>48.8658424320023</v>
       </c>
       <c r="H6" t="n">
-        <v>57.5729328851664</v>
+        <v>84.010356288206</v>
       </c>
     </row>
     <row r="7">
@@ -567,25 +570,25 @@
         <v>13</v>
       </c>
       <c r="B7" t="n">
-        <v>287</v>
+        <v>247</v>
       </c>
       <c r="C7" t="n">
-        <v>4012.29965156794</v>
+        <v>4285.68825910931</v>
       </c>
       <c r="D7" t="n">
-        <v>1549.7222994326</v>
+        <v>2472.06516561117</v>
       </c>
       <c r="E7" t="n">
-        <v>6474.87700370329</v>
+        <v>6099.31135260746</v>
       </c>
       <c r="F7" t="n">
-        <v>23.8659014613487</v>
+        <v>51.2030403669678</v>
       </c>
       <c r="G7" t="n">
-        <v>6.84649947783738</v>
+        <v>31.7394759675061</v>
       </c>
       <c r="H7" t="n">
-        <v>43.5962958057882</v>
+        <v>73.5422070591352</v>
       </c>
     </row>
     <row r="8">
@@ -593,25 +596,25 @@
         <v>14</v>
       </c>
       <c r="B8" t="n">
-        <v>184</v>
+        <v>140</v>
       </c>
       <c r="C8" t="n">
-        <v>5905.4402173913</v>
+        <v>5383.36428571429</v>
       </c>
       <c r="D8" t="n">
-        <v>2889.42549041559</v>
+        <v>2827.14649923311</v>
       </c>
       <c r="E8" t="n">
-        <v>8921.45494436702</v>
+        <v>7939.58207219546</v>
       </c>
       <c r="F8" t="n">
-        <v>44.8845316038222</v>
+        <v>68.3921251544791</v>
       </c>
       <c r="G8" t="n">
-        <v>21.41121023058</v>
+        <v>38.6970089929833</v>
       </c>
       <c r="H8" t="n">
-        <v>72.8961226742783</v>
+        <v>104.444984213584</v>
       </c>
     </row>
     <row r="9">
@@ -619,25 +622,25 @@
         <v>15</v>
       </c>
       <c r="B9" t="n">
-        <v>473</v>
+        <v>392</v>
       </c>
       <c r="C9" t="n">
-        <v>5941.61733615222</v>
+        <v>4379.93112244898</v>
       </c>
       <c r="D9" t="n">
-        <v>4306.84686242448</v>
+        <v>3148.56358469062</v>
       </c>
       <c r="E9" t="n">
-        <v>7576.38780987996</v>
+        <v>5611.29866020734</v>
       </c>
       <c r="F9" t="n">
-        <v>54.4490455677735</v>
+        <v>67.368130068063</v>
       </c>
       <c r="G9" t="n">
-        <v>38.4040986642213</v>
+        <v>50.3133693989219</v>
       </c>
       <c r="H9" t="n">
-        <v>72.3540553135569</v>
+        <v>86.3579472304809</v>
       </c>
     </row>
     <row r="10">
@@ -645,25 +648,25 @@
         <v>16</v>
       </c>
       <c r="B10" t="n">
-        <v>543</v>
+        <v>454</v>
       </c>
       <c r="C10" t="n">
-        <v>7767.69244935543</v>
+        <v>7023.04185022026</v>
       </c>
       <c r="D10" t="n">
-        <v>6035.88844322261</v>
+        <v>5646.598832422</v>
       </c>
       <c r="E10" t="n">
-        <v>9499.49645548826</v>
+        <v>8399.48486801854</v>
       </c>
       <c r="F10" t="n">
-        <v>63.5287467489932</v>
+        <v>87.2034416652225</v>
       </c>
       <c r="G10" t="n">
-        <v>46.6978910518555</v>
+        <v>69.9099582948445</v>
       </c>
       <c r="H10" t="n">
-        <v>82.2906302302846</v>
+        <v>106.257060639675</v>
       </c>
     </row>
     <row r="11">
@@ -671,25 +674,25 @@
         <v>17</v>
       </c>
       <c r="B11" t="n">
-        <v>509</v>
+        <v>417</v>
       </c>
       <c r="C11" t="n">
-        <v>9986.43418467583</v>
+        <v>9736.36211031175</v>
       </c>
       <c r="D11" t="n">
-        <v>7968.512908009</v>
+        <v>8136.12689722172</v>
       </c>
       <c r="E11" t="n">
-        <v>12004.3554613427</v>
+        <v>11336.5973234018</v>
       </c>
       <c r="F11" t="n">
-        <v>84.629022437725</v>
+        <v>127.167474230522</v>
       </c>
       <c r="G11" t="n">
-        <v>63.4141853892643</v>
+        <v>106.403026976817</v>
       </c>
       <c r="H11" t="n">
-        <v>108.598022534642</v>
+        <v>150.020855334022</v>
       </c>
     </row>
     <row r="12">
@@ -697,25 +700,25 @@
         <v>18</v>
       </c>
       <c r="B12" t="n">
-        <v>680</v>
+        <v>592</v>
       </c>
       <c r="C12" t="n">
-        <v>4695.12058823529</v>
+        <v>3477.55236486487</v>
       </c>
       <c r="D12" t="n">
-        <v>3482.82323385664</v>
+        <v>2587.63700177929</v>
       </c>
       <c r="E12" t="n">
-        <v>5907.41794261395</v>
+        <v>4367.46772795044</v>
       </c>
       <c r="F12" t="n">
-        <v>41.2873374027604</v>
+        <v>51.2598517950677</v>
       </c>
       <c r="G12" t="n">
-        <v>29.1788613355816</v>
+        <v>39.4830567718202</v>
       </c>
       <c r="H12" t="n">
-        <v>54.5307916788627</v>
+        <v>64.0309819313352</v>
       </c>
     </row>
     <row r="13">
@@ -723,25 +726,25 @@
         <v>19</v>
       </c>
       <c r="B13" t="n">
-        <v>328</v>
+        <v>267</v>
       </c>
       <c r="C13" t="n">
-        <v>9635.97256097561</v>
+        <v>8593.22846441948</v>
       </c>
       <c r="D13" t="n">
-        <v>7277.18306734735</v>
+        <v>6870.42788015657</v>
       </c>
       <c r="E13" t="n">
-        <v>11994.7620546039</v>
+        <v>10316.0290486824</v>
       </c>
       <c r="F13" t="n">
-        <v>86.141824160658</v>
+        <v>95.349073603191</v>
       </c>
       <c r="G13" t="n">
-        <v>60.8955424557884</v>
+        <v>74.6299266386883</v>
       </c>
       <c r="H13" t="n">
-        <v>115.349525369096</v>
+        <v>118.526465034719</v>
       </c>
     </row>
     <row r="14">
@@ -749,25 +752,51 @@
         <v>20</v>
       </c>
       <c r="B14" t="n">
-        <v>221</v>
+        <v>170</v>
       </c>
       <c r="C14" t="n">
-        <v>5363.75113122172</v>
+        <v>7376.07647058824</v>
       </c>
       <c r="D14" t="n">
-        <v>2704.66743607948</v>
+        <v>5262.32772055414</v>
       </c>
       <c r="E14" t="n">
-        <v>8022.83482636396</v>
+        <v>9489.82522062233</v>
       </c>
       <c r="F14" t="n">
-        <v>50.8517269867928</v>
+        <v>110.185676953546</v>
       </c>
       <c r="G14" t="n">
-        <v>29.0932322739088</v>
+        <v>78.4682011470801</v>
       </c>
       <c r="H14" t="n">
-        <v>76.2775873998869</v>
+        <v>147.540001593967</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="n">
+        <v>62</v>
+      </c>
+      <c r="C15" t="n">
+        <v>8144.58064516129</v>
+      </c>
+      <c r="D15" t="n">
+        <v>3732.43330338389</v>
+      </c>
+      <c r="E15" t="n">
+        <v>12556.7279869387</v>
+      </c>
+      <c r="F15" t="n">
+        <v>133.431450505943</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.458296605095265</v>
+      </c>
+      <c r="H15" t="n">
+        <v>244.574433398863</v>
       </c>
     </row>
   </sheetData>

</xml_diff>